<commit_message>
Ultimos cambios con la bd
</commit_message>
<xml_diff>
--- a/excel/aceites.xlsx
+++ b/excel/aceites.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>FOLIO</t>
   </si>
@@ -36,7 +36,10 @@
     <t>Cant. Aceites</t>
   </si>
   <si>
-    <t>2025-01-12</t>
+    <t>precio</t>
+  </si>
+  <si>
+    <t>folio</t>
   </si>
   <si>
     <t>2025-01-13</t>
@@ -63,9 +66,6 @@
     <t>2025-01-23</t>
   </si>
   <si>
-    <t>planta</t>
-  </si>
-  <si>
     <t>2025-01-24</t>
   </si>
   <si>
@@ -93,30 +93,59 @@
     <t>2025-02-05</t>
   </si>
   <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>folio</t>
+    <t>MOTOS</t>
+  </si>
+  <si>
+    <t>SUM Motos</t>
+  </si>
+  <si>
+    <t>GASTO</t>
+  </si>
+  <si>
+    <t>administrativo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -131,8 +160,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,40 +470,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2" s="2">
+        <v>45669</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -478,16 +524,28 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="3">
+        <v>93</v>
+      </c>
+      <c r="G2">
+        <f t="array" ref="G2">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G1, $C$2:$C$100), 0)), "")</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f>COUNTIF($C$2:$C$100, G2)</f>
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <f>SUMIF($C$2:$C$100, G2, $E$2:$E$100)</f>
+        <v>744</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -495,16 +553,28 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="3">
+        <v>93</v>
+      </c>
+      <c r="G3">
+        <f t="array" ref="G3">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G2, $C$2:$C$100), 0)), "")</f>
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <f>COUNTIF($C$2:$C$100, G3)</f>
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I12" si="0">SUMIF($C$2:$C$100, G3, $E$2:$E$100)</f>
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -512,16 +582,28 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="3">
+        <v>93</v>
+      </c>
+      <c r="G4">
+        <f t="array" ref="G4">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G3, $C$2:$C$100), 0)), "")</f>
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <f>COUNTIF($C$2:$C$100, G4)</f>
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>19</v>
@@ -529,16 +611,28 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="3">
+        <v>93</v>
+      </c>
+      <c r="G5">
+        <f t="array" ref="G5">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G4, $C$2:$C$100), 0)), "")</f>
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <f>COUNTIF($C$2:$C$100, G5)</f>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -546,16 +640,28 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="3">
+        <v>93</v>
+      </c>
+      <c r="G6">
+        <f t="array" ref="G6">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G5, $C$2:$C$100), 0)), "")</f>
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <f>COUNTIF($C$2:$C$100, G6)</f>
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>16</v>
@@ -563,16 +669,28 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="3">
+        <v>93</v>
+      </c>
+      <c r="G7">
+        <f t="array" ref="G7">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G6, $C$2:$C$100), 0)), "")</f>
+        <v>16</v>
+      </c>
+      <c r="H7">
+        <f>COUNTIF($C$2:$C$100, G7)</f>
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -580,16 +698,28 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="3">
+        <v>93</v>
+      </c>
+      <c r="G8">
+        <f t="array" ref="G8">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G7, $C$2:$C$100), 0)), "")</f>
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <f>COUNTIF($C$2:$C$100, G8)</f>
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -597,16 +727,28 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="3">
+        <v>93</v>
+      </c>
+      <c r="G9">
+        <f t="array" ref="G9">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G8, $C$2:$C$100), 0)), "")</f>
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <f>COUNTIF($C$2:$C$100, G9)</f>
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -614,16 +756,28 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="3">
+        <v>93</v>
+      </c>
+      <c r="G10">
+        <f t="array" ref="G10">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G9, $C$2:$C$100), 0)), "")</f>
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <f>COUNTIF($C$2:$C$100, G10)</f>
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -631,16 +785,28 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="3">
+        <v>93</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="array" ref="G11">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G10, $C$2:$C$100), 0)), "")</f>
+        <v>administrativo</v>
+      </c>
+      <c r="H11">
+        <f>COUNTIF($C$2:$C$100, G11)</f>
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -648,16 +814,28 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="3">
+        <v>93</v>
+      </c>
+      <c r="G12">
+        <f t="array" ref="G12">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G11, $C$2:$C$100), 0)), "")</f>
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <f>COUNTIF($C$2:$C$100, G12)</f>
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -665,16 +843,16 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -682,16 +860,16 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <v>15</v>
@@ -699,16 +877,16 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -716,7 +894,7 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <v>93</v>
       </c>
     </row>
@@ -725,7 +903,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -733,7 +911,7 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="3">
         <v>93</v>
       </c>
     </row>
@@ -742,7 +920,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18">
         <v>10</v>
@@ -750,7 +928,7 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <v>93</v>
       </c>
     </row>
@@ -759,7 +937,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19">
         <v>14</v>
@@ -767,7 +945,7 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="3">
         <v>93</v>
       </c>
     </row>
@@ -776,7 +954,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -784,7 +962,7 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="3">
         <v>93</v>
       </c>
     </row>
@@ -793,15 +971,15 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
         <v>13</v>
       </c>
+      <c r="C21" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="3">
         <v>93</v>
       </c>
     </row>
@@ -810,7 +988,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C22">
         <v>10</v>
@@ -818,7 +996,7 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="3">
         <v>93</v>
       </c>
     </row>
@@ -835,7 +1013,7 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="3">
         <v>93</v>
       </c>
     </row>
@@ -852,7 +1030,7 @@
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="3">
         <v>93</v>
       </c>
     </row>
@@ -869,7 +1047,7 @@
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="3">
         <v>93</v>
       </c>
     </row>
@@ -886,7 +1064,7 @@
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="3">
         <v>93</v>
       </c>
     </row>
@@ -903,7 +1081,7 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="3">
         <v>93</v>
       </c>
     </row>
@@ -920,7 +1098,7 @@
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="3">
         <v>93</v>
       </c>
     </row>
@@ -937,7 +1115,7 @@
       <c r="D29">
         <v>1</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="3">
         <v>93</v>
       </c>
     </row>
@@ -954,7 +1132,7 @@
       <c r="D30">
         <v>1</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="3">
         <v>93</v>
       </c>
     </row>
@@ -971,7 +1149,7 @@
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="3">
         <v>93</v>
       </c>
     </row>
@@ -988,7 +1166,7 @@
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="3">
         <v>93</v>
       </c>
     </row>
@@ -1005,7 +1183,7 @@
       <c r="D33">
         <v>1</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="3">
         <v>93</v>
       </c>
     </row>
@@ -1022,7 +1200,7 @@
       <c r="D34">
         <v>1</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="3">
         <v>93</v>
       </c>
     </row>
@@ -1039,7 +1217,7 @@
       <c r="D35">
         <v>1</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="3">
         <v>93</v>
       </c>
     </row>
@@ -1056,7 +1234,7 @@
       <c r="D36">
         <v>1</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="3">
         <v>93</v>
       </c>
     </row>
@@ -1068,12 +1246,12 @@
         <v>20</v>
       </c>
       <c r="C37">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="3">
         <v>93</v>
       </c>
     </row>
@@ -1085,12 +1263,12 @@
         <v>20</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="3">
         <v>93</v>
       </c>
     </row>
@@ -1102,12 +1280,12 @@
         <v>21</v>
       </c>
       <c r="C39">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="3">
         <v>93</v>
       </c>
     </row>
@@ -1119,17 +1297,35 @@
         <v>22</v>
       </c>
       <c r="C40">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>54</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3">
         <v>93</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:I1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="187" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nuevo con bootstrap y mas
</commit_message>
<xml_diff>
--- a/excel/aceites.xlsx
+++ b/excel/aceites.xlsx
@@ -1,45 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\AceitesSufa\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja1'!$A$1:$L$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>FECHA</t>
+  </si>
+  <si>
+    <t>Num. Moto</t>
+  </si>
+  <si>
+    <t>Cant. Aceites</t>
+  </si>
+  <si>
+    <t>PRECIO</t>
+  </si>
   <si>
     <t>FOLIO</t>
   </si>
   <si>
-    <t>FECHA</t>
-  </si>
-  <si>
-    <t>Num. Moto</t>
-  </si>
-  <si>
-    <t>Cant. Aceites</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>folio</t>
+    <t>MOTOS</t>
+  </si>
+  <si>
+    <t>SUM Motos</t>
+  </si>
+  <si>
+    <t>GASTO</t>
+  </si>
+  <si>
+    <t>2025-01-12</t>
+  </si>
+  <si>
+    <t>IWAED389096</t>
   </si>
   <si>
     <t>2025-01-13</t>
@@ -57,15 +67,27 @@
     <t>2025-01-19</t>
   </si>
   <si>
+    <t>IWAED389456</t>
+  </si>
+  <si>
+    <t>oswi</t>
+  </si>
+  <si>
     <t>2025-01-21</t>
   </si>
   <si>
+    <t>planta</t>
+  </si>
+  <si>
     <t>2025-01-22</t>
   </si>
   <si>
     <t>2025-01-23</t>
   </si>
   <si>
+    <t>IWAED389881</t>
+  </si>
+  <si>
     <t>2025-01-24</t>
   </si>
   <si>
@@ -81,6 +103,9 @@
     <t>2025-01-31</t>
   </si>
   <si>
+    <t>IWAED390612</t>
+  </si>
+  <si>
     <t>2025-02-01</t>
   </si>
   <si>
@@ -93,44 +118,54 @@
     <t>2025-02-05</t>
   </si>
   <si>
-    <t>MOTOS</t>
-  </si>
-  <si>
-    <t>SUM Motos</t>
-  </si>
-  <si>
-    <t>GASTO</t>
-  </si>
-  <si>
-    <t>administrativo</t>
+    <t>2025-02-06</t>
+  </si>
+  <si>
+    <t>IWAED390887</t>
+  </si>
+  <si>
+    <t>2025-02-07</t>
+  </si>
+  <si>
+    <t>2025-02-08</t>
+  </si>
+  <si>
+    <t>2025-02-09</t>
+  </si>
+  <si>
+    <t>2025-02-10</t>
+  </si>
+  <si>
+    <t>2025-02-11</t>
+  </si>
+  <si>
+    <t>2025-02-12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -143,8 +178,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF2E75B5"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -160,26 +195,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+  <cellXfs count="3">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -469,54 +498,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="9.140625" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="true" style="0"/>
+    <col min="6" max="6" width="18" customWidth="true" style="0"/>
+    <col min="9" max="9" width="11.85546875" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G1" s="2"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>45669</v>
+      <c r="B2" t="s">
+        <v>9</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -524,28 +560,28 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="3">
-        <v>93</v>
-      </c>
-      <c r="G2">
-        <f t="array" ref="G2">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G1, $C$2:$C$100), 0)), "")</f>
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <f>COUNTIF($C$2:$C$100, G2)</f>
+      <c r="E2">
+        <v>93</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
         <v>8</v>
       </c>
-      <c r="I2">
-        <f>SUMIF($C$2:$C$100, G2, $E$2:$E$100)</f>
+      <c r="L2">
         <v>744</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -553,28 +589,28 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="3">
-        <v>93</v>
-      </c>
-      <c r="G3">
-        <f t="array" ref="G3">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G2, $C$2:$C$100), 0)), "")</f>
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <f>COUNTIF($C$2:$C$100, G3)</f>
+      <c r="E3">
+        <v>93</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
         <v>15</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I12" si="0">SUMIF($C$2:$C$100, G3, $E$2:$E$100)</f>
+      <c r="L3">
         <v>1395</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -582,28 +618,28 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="3">
-        <v>93</v>
-      </c>
-      <c r="G4">
-        <f t="array" ref="G4">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G3, $C$2:$C$100), 0)), "")</f>
+      <c r="E4">
+        <v>93</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4">
         <v>12</v>
       </c>
-      <c r="H4">
-        <f>COUNTIF($C$2:$C$100, G4)</f>
+      <c r="K4">
         <v>2</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
+      <c r="L4">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>19</v>
@@ -611,28 +647,28 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
-        <v>93</v>
-      </c>
-      <c r="G5">
-        <f t="array" ref="G5">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G4, $C$2:$C$100), 0)), "")</f>
-        <v>19</v>
-      </c>
-      <c r="H5">
-        <f>COUNTIF($C$2:$C$100, G5)</f>
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>93</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>14</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -640,28 +676,28 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="3">
-        <v>93</v>
-      </c>
-      <c r="G6">
-        <f t="array" ref="G6">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G5, $C$2:$C$100), 0)), "")</f>
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <f>COUNTIF($C$2:$C$100, G6)</f>
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>93</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>15</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>16</v>
@@ -669,28 +705,28 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="3">
-        <v>93</v>
-      </c>
-      <c r="G7">
-        <f t="array" ref="G7">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G6, $C$2:$C$100), 0)), "")</f>
+      <c r="E7">
+        <v>93</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7">
         <v>16</v>
       </c>
-      <c r="H7">
-        <f>COUNTIF($C$2:$C$100, G7)</f>
+      <c r="K7">
         <v>2</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
+      <c r="L7">
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -698,28 +734,28 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="3">
-        <v>93</v>
-      </c>
-      <c r="G8">
-        <f t="array" ref="G8">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G7, $C$2:$C$100), 0)), "")</f>
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <f>COUNTIF($C$2:$C$100, G8)</f>
-        <v>2</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>93</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>19</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -727,28 +763,28 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="3">
-        <v>93</v>
-      </c>
-      <c r="G9">
-        <f t="array" ref="G9">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G8, $C$2:$C$100), 0)), "")</f>
-        <v>15</v>
-      </c>
-      <c r="H9">
-        <f>COUNTIF($C$2:$C$100, G9)</f>
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>93</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -756,57 +792,57 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" s="3">
-        <v>93</v>
-      </c>
-      <c r="G10">
-        <f t="array" ref="G10">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G9, $C$2:$C$100), 0)), "")</f>
+      <c r="E10">
+        <v>93</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="H10">
-        <f>COUNTIF($C$2:$C$100, G10)</f>
-        <v>2</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>186</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" s="3">
-        <v>93</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="array" ref="G11">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G10, $C$2:$C$100), 0)), "")</f>
-        <v>administrativo</v>
-      </c>
-      <c r="H11">
-        <f>COUNTIF($C$2:$C$100, G11)</f>
-        <v>2</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>186</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>93</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -814,28 +850,28 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" s="3">
-        <v>93</v>
-      </c>
-      <c r="G12">
-        <f t="array" ref="G12">IFERROR(INDEX($C$2:$C$100, MATCH(0, COUNTIF($G$1:G11, $C$2:$C$100), 0)), "")</f>
-        <v>6</v>
-      </c>
-      <c r="H12">
-        <f>COUNTIF($C$2:$C$100, G12)</f>
-        <v>3</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>279</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>93</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -843,16 +879,28 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>93</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -860,16 +908,19 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>93</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>15</v>
@@ -877,16 +928,19 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>93</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -894,16 +948,19 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>93</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -911,16 +968,19 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>93</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>10</v>
@@ -928,16 +988,19 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>93</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>14</v>
@@ -945,16 +1008,19 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>93</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -962,33 +1028,39 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>93</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>93</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>10</v>
@@ -996,16 +1068,19 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>93</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C23">
         <v>6</v>
@@ -1013,16 +1088,19 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>93</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>10</v>
@@ -1030,16 +1108,19 @@
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="E24" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>93</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -1047,16 +1128,19 @@
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="E25" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>93</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C26">
         <v>6</v>
@@ -1064,16 +1148,19 @@
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>93</v>
+      </c>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1081,16 +1168,19 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>93</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C28">
         <v>10</v>
@@ -1098,16 +1188,19 @@
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="E28" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>93</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C29">
         <v>14</v>
@@ -1115,16 +1208,19 @@
       <c r="D29">
         <v>1</v>
       </c>
-      <c r="E29" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>93</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1132,16 +1228,19 @@
       <c r="D30">
         <v>1</v>
       </c>
-      <c r="E30" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>93</v>
+      </c>
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C31">
         <v>10</v>
@@ -1149,16 +1248,19 @@
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>93</v>
+      </c>
+      <c r="F31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32">
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C32">
         <v>10</v>
@@ -1166,16 +1268,19 @@
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="E32" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>93</v>
+      </c>
+      <c r="F32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C33">
         <v>10</v>
@@ -1183,16 +1288,19 @@
       <c r="D33">
         <v>1</v>
       </c>
-      <c r="E33" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>93</v>
+      </c>
+      <c r="F33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34">
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C34">
         <v>12</v>
@@ -1200,16 +1308,19 @@
       <c r="D34">
         <v>1</v>
       </c>
-      <c r="E34" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>93</v>
+      </c>
+      <c r="F34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35">
         <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -1217,16 +1328,19 @@
       <c r="D35">
         <v>1</v>
       </c>
-      <c r="E35" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>93</v>
+      </c>
+      <c r="F35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36">
         <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1234,16 +1348,19 @@
       <c r="D36">
         <v>1</v>
       </c>
-      <c r="E36" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>93</v>
+      </c>
+      <c r="F36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37">
         <v>50</v>
       </c>
       <c r="B37" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1251,16 +1368,19 @@
       <c r="D37">
         <v>1</v>
       </c>
-      <c r="E37" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>93</v>
+      </c>
+      <c r="F37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38">
         <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C38">
         <v>10</v>
@@ -1268,16 +1388,19 @@
       <c r="D38">
         <v>1</v>
       </c>
-      <c r="E38" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>93</v>
+      </c>
+      <c r="F38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39">
         <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C39">
         <v>6</v>
@@ -1285,16 +1408,19 @@
       <c r="D39">
         <v>1</v>
       </c>
-      <c r="E39" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>93</v>
+      </c>
+      <c r="F39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40">
         <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1302,30 +1428,228 @@
       <c r="D40">
         <v>1</v>
       </c>
-      <c r="E40" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>93</v>
+      </c>
+      <c r="F40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41">
         <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="C41" t="s">
+        <v>17</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
-      <c r="E41" s="3">
-        <v>93</v>
+      <c r="E41">
+        <v>93</v>
+      </c>
+      <c r="F41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42">
+        <v>65</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>95</v>
+      </c>
+      <c r="F42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43">
+        <v>66</v>
+      </c>
+      <c r="B43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43">
+        <v>14</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>95</v>
+      </c>
+      <c r="F43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44">
+        <v>67</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44">
+        <v>16</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>95</v>
+      </c>
+      <c r="F44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45">
+        <v>68</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>95</v>
+      </c>
+      <c r="F45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46">
+        <v>69</v>
+      </c>
+      <c r="B46" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>95</v>
+      </c>
+      <c r="F46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47">
+        <v>70</v>
+      </c>
+      <c r="B47" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>95</v>
+      </c>
+      <c r="F47" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48">
+        <v>71</v>
+      </c>
+      <c r="B48" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>95</v>
+      </c>
+      <c r="F48" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49">
+        <v>72</v>
+      </c>
+      <c r="B49" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50">
+        <v>73</v>
+      </c>
+      <c r="B50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51">
+        <v>74</v>
+      </c>
+      <c r="B51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51">
+        <v>6</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
+  <autoFilter ref="A1:L1"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="187" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
+  <pageSetup paperSize="187" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId1ps"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
diseño de la gpaina aceites
</commit_message>
<xml_diff>
--- a/excel/aceites.xlsx
+++ b/excel/aceites.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
   <si>
     <t>ID</t>
   </si>
@@ -70,54 +70,54 @@
     <t>IWAED389456</t>
   </si>
   <si>
+    <t>2025-01-21</t>
+  </si>
+  <si>
+    <t>2025-01-22</t>
+  </si>
+  <si>
+    <t>2025-01-23</t>
+  </si>
+  <si>
+    <t>planta</t>
+  </si>
+  <si>
+    <t>IWAED389881</t>
+  </si>
+  <si>
+    <t>2025-01-24</t>
+  </si>
+  <si>
+    <t>2025-01-25</t>
+  </si>
+  <si>
+    <t>2025-01-27</t>
+  </si>
+  <si>
+    <t>2025-01-29</t>
+  </si>
+  <si>
+    <t>2025-01-31</t>
+  </si>
+  <si>
+    <t>IWAED390612</t>
+  </si>
+  <si>
+    <t>2025-02-01</t>
+  </si>
+  <si>
+    <t>2025-02-03</t>
+  </si>
+  <si>
+    <t>2025-02-02</t>
+  </si>
+  <si>
+    <t>2025-02-05</t>
+  </si>
+  <si>
     <t>oswi</t>
   </si>
   <si>
-    <t>2025-01-21</t>
-  </si>
-  <si>
-    <t>planta</t>
-  </si>
-  <si>
-    <t>2025-01-22</t>
-  </si>
-  <si>
-    <t>2025-01-23</t>
-  </si>
-  <si>
-    <t>IWAED389881</t>
-  </si>
-  <si>
-    <t>2025-01-24</t>
-  </si>
-  <si>
-    <t>2025-01-25</t>
-  </si>
-  <si>
-    <t>2025-01-27</t>
-  </si>
-  <si>
-    <t>2025-01-29</t>
-  </si>
-  <si>
-    <t>2025-01-31</t>
-  </si>
-  <si>
-    <t>IWAED390612</t>
-  </si>
-  <si>
-    <t>2025-02-01</t>
-  </si>
-  <si>
-    <t>2025-02-03</t>
-  </si>
-  <si>
-    <t>2025-02-02</t>
-  </si>
-  <si>
-    <t>2025-02-05</t>
-  </si>
-  <si>
     <t>2025-02-06</t>
   </si>
   <si>
@@ -140,6 +140,144 @@
   </si>
   <si>
     <t>2025-02-12</t>
+  </si>
+  <si>
+    <t>2025-02-13</t>
+  </si>
+  <si>
+    <t>IWAED391789</t>
+  </si>
+  <si>
+    <t>2025-02-17</t>
+  </si>
+  <si>
+    <t>2025-02-19</t>
+  </si>
+  <si>
+    <t>2025-02-14</t>
+  </si>
+  <si>
+    <t>2025-02-20</t>
+  </si>
+  <si>
+    <t>IWAED391908</t>
+  </si>
+  <si>
+    <t>2025-02-21</t>
+  </si>
+  <si>
+    <t>2025-02-24</t>
+  </si>
+  <si>
+    <t>2025-02-26</t>
+  </si>
+  <si>
+    <t>2025-02-27</t>
+  </si>
+  <si>
+    <t>2025-03-03</t>
+  </si>
+  <si>
+    <t>2025-03-06</t>
+  </si>
+  <si>
+    <t>IWAED392982</t>
+  </si>
+  <si>
+    <t>2025-03-10</t>
+  </si>
+  <si>
+    <t>2025-03-12</t>
+  </si>
+  <si>
+    <t>2025-03-13</t>
+  </si>
+  <si>
+    <t>2025-03-16</t>
+  </si>
+  <si>
+    <t>2025-03-17</t>
+  </si>
+  <si>
+    <t>2025-03-20</t>
+  </si>
+  <si>
+    <t>2025-03-22</t>
+  </si>
+  <si>
+    <t>2025-04-22</t>
+  </si>
+  <si>
+    <t>2025-03-26</t>
+  </si>
+  <si>
+    <t>2025-03-29</t>
+  </si>
+  <si>
+    <t>IWAED394557</t>
+  </si>
+  <si>
+    <t>2025-03-30</t>
+  </si>
+  <si>
+    <t>2025-04-30</t>
+  </si>
+  <si>
+    <t>2025-04-08</t>
+  </si>
+  <si>
+    <t>2025-04-07</t>
+  </si>
+  <si>
+    <t>2025-04-09</t>
+  </si>
+  <si>
+    <t>2025-04-12</t>
+  </si>
+  <si>
+    <t>2025-04-29</t>
+  </si>
+  <si>
+    <t>2025-04-15</t>
+  </si>
+  <si>
+    <t>IWAED395730</t>
+  </si>
+  <si>
+    <t>2025-04-18</t>
+  </si>
+  <si>
+    <t>2025-04-23</t>
+  </si>
+  <si>
+    <t>2025-04-24</t>
+  </si>
+  <si>
+    <t>2025-04-26</t>
+  </si>
+  <si>
+    <t>2025-04-27</t>
+  </si>
+  <si>
+    <t>IWAED396530</t>
+  </si>
+  <si>
+    <t>2025-05-01</t>
+  </si>
+  <si>
+    <t>2025-05-03</t>
+  </si>
+  <si>
+    <t>2025-05-05</t>
+  </si>
+  <si>
+    <t>2025-05-07</t>
+  </si>
+  <si>
+    <t>2025-05-10</t>
+  </si>
+  <si>
+    <t>2025-05-12</t>
   </si>
 </sst>
 </file>
@@ -502,7 +640,7 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="N8" sqref="N8"/>
@@ -570,10 +708,10 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="L2">
-        <v>744</v>
+        <v>2169</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -599,10 +737,10 @@
         <v>10</v>
       </c>
       <c r="K3">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="L3">
-        <v>1395</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -628,10 +766,10 @@
         <v>12</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L4">
-        <v>186</v>
+        <v>566</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -657,10 +795,10 @@
         <v>14</v>
       </c>
       <c r="K5">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="L5">
-        <v>186</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -715,10 +853,10 @@
         <v>16</v>
       </c>
       <c r="K7">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L7">
-        <v>186</v>
+        <v>851</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -741,13 +879,13 @@
         <v>10</v>
       </c>
       <c r="J8">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L8">
-        <v>93</v>
+        <v>570</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -770,13 +908,13 @@
         <v>10</v>
       </c>
       <c r="J9">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="K9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L9">
-        <v>186</v>
+        <v>663</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -799,13 +937,13 @@
         <v>10</v>
       </c>
       <c r="J10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L10">
-        <v>186</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -828,13 +966,13 @@
         <v>10</v>
       </c>
       <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
         <v>6</v>
       </c>
-      <c r="K11">
-        <v>3</v>
-      </c>
       <c r="L11">
-        <v>279</v>
+        <v>566</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -856,14 +994,14 @@
       <c r="F12" t="s">
         <v>16</v>
       </c>
-      <c r="J12" t="s">
-        <v>17</v>
+      <c r="J12">
+        <v>5</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L12">
-        <v>93</v>
+        <v>471</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -871,7 +1009,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -885,14 +1023,14 @@
       <c r="F13" t="s">
         <v>16</v>
       </c>
-      <c r="J13" t="s">
-        <v>19</v>
+      <c r="J13">
+        <v>6</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L13">
-        <v>93</v>
+        <v>564</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -900,7 +1038,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -913,6 +1051,15 @@
       </c>
       <c r="F14" t="s">
         <v>16</v>
+      </c>
+      <c r="J14">
+        <v>9</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -920,7 +1067,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>15</v>
@@ -933,6 +1080,15 @@
       </c>
       <c r="F15" t="s">
         <v>16</v>
+      </c>
+      <c r="J15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -940,7 +1096,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -953,6 +1109,15 @@
       </c>
       <c r="F16" t="s">
         <v>16</v>
+      </c>
+      <c r="J16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -960,7 +1125,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -980,7 +1145,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>10</v>
@@ -1000,7 +1165,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>14</v>
@@ -1020,7 +1185,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1040,10 +1205,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1060,19 +1225,19 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>93</v>
+      </c>
+      <c r="F22" t="s">
         <v>21</v>
-      </c>
-      <c r="C22">
-        <v>10</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>93</v>
-      </c>
-      <c r="F22" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1080,7 +1245,7 @@
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>6</v>
@@ -1092,7 +1257,7 @@
         <v>93</v>
       </c>
       <c r="F23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1100,7 +1265,7 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24">
         <v>10</v>
@@ -1112,7 +1277,7 @@
         <v>93</v>
       </c>
       <c r="F24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1120,7 +1285,7 @@
         <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -1132,7 +1297,7 @@
         <v>93</v>
       </c>
       <c r="F25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1140,7 +1305,7 @@
         <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26">
         <v>6</v>
@@ -1152,7 +1317,7 @@
         <v>93</v>
       </c>
       <c r="F26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1160,7 +1325,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1172,7 +1337,7 @@
         <v>93</v>
       </c>
       <c r="F27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1180,7 +1345,7 @@
         <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28">
         <v>10</v>
@@ -1192,7 +1357,7 @@
         <v>93</v>
       </c>
       <c r="F28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1200,7 +1365,7 @@
         <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29">
         <v>14</v>
@@ -1212,7 +1377,7 @@
         <v>93</v>
       </c>
       <c r="F29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1220,7 +1385,7 @@
         <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1232,7 +1397,7 @@
         <v>93</v>
       </c>
       <c r="F30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1240,7 +1405,7 @@
         <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31">
         <v>10</v>
@@ -1252,7 +1417,7 @@
         <v>93</v>
       </c>
       <c r="F31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1260,19 +1425,19 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>93</v>
+      </c>
+      <c r="F32" t="s">
         <v>27</v>
-      </c>
-      <c r="C32">
-        <v>10</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <v>93</v>
-      </c>
-      <c r="F32" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1280,19 +1445,19 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>93</v>
+      </c>
+      <c r="F33" t="s">
         <v>27</v>
-      </c>
-      <c r="C33">
-        <v>10</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>93</v>
-      </c>
-      <c r="F33" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1300,7 +1465,7 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C34">
         <v>12</v>
@@ -1312,7 +1477,7 @@
         <v>93</v>
       </c>
       <c r="F34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1320,7 +1485,7 @@
         <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -1332,7 +1497,7 @@
         <v>93</v>
       </c>
       <c r="F35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1340,7 +1505,7 @@
         <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1352,7 +1517,7 @@
         <v>93</v>
       </c>
       <c r="F36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1360,7 +1525,7 @@
         <v>50</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1372,7 +1537,7 @@
         <v>93</v>
       </c>
       <c r="F37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1380,7 +1545,7 @@
         <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38">
         <v>10</v>
@@ -1392,7 +1557,7 @@
         <v>93</v>
       </c>
       <c r="F38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -1400,7 +1565,7 @@
         <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39">
         <v>6</v>
@@ -1412,7 +1577,7 @@
         <v>93</v>
       </c>
       <c r="F39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -1420,7 +1585,7 @@
         <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1432,7 +1597,7 @@
         <v>93</v>
       </c>
       <c r="F40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -1440,11 +1605,11 @@
         <v>54</v>
       </c>
       <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" t="s">
         <v>32</v>
       </c>
-      <c r="C41" t="s">
-        <v>17</v>
-      </c>
       <c r="D41">
         <v>1</v>
       </c>
@@ -1452,7 +1617,7 @@
         <v>93</v>
       </c>
       <c r="F41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -1611,6 +1776,9 @@
       <c r="E49">
         <v>95</v>
       </c>
+      <c r="F49" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="50" spans="1:12">
       <c r="A50">
@@ -1628,6 +1796,9 @@
       <c r="E50">
         <v>95</v>
       </c>
+      <c r="F50" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51">
@@ -1644,6 +1815,1189 @@
       </c>
       <c r="E51">
         <v>95</v>
+      </c>
+      <c r="F51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52">
+        <v>75</v>
+      </c>
+      <c r="B52" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52">
+        <v>10</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>95</v>
+      </c>
+      <c r="F52" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53">
+        <v>77</v>
+      </c>
+      <c r="B53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>95</v>
+      </c>
+      <c r="F53" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54">
+        <v>78</v>
+      </c>
+      <c r="B54" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54">
+        <v>14</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>95</v>
+      </c>
+      <c r="F54" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55">
+        <v>79</v>
+      </c>
+      <c r="B55" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55">
+        <v>19</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>95</v>
+      </c>
+      <c r="F55" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56">
+        <v>80</v>
+      </c>
+      <c r="B56" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>95</v>
+      </c>
+      <c r="F56" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57">
+        <v>81</v>
+      </c>
+      <c r="B57" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57">
+        <v>19</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>95</v>
+      </c>
+      <c r="F57" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58">
+        <v>82</v>
+      </c>
+      <c r="B58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C58">
+        <v>14</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>95</v>
+      </c>
+      <c r="F58" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59">
+        <v>83</v>
+      </c>
+      <c r="B59" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59">
+        <v>16</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>95</v>
+      </c>
+      <c r="F59" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60">
+        <v>84</v>
+      </c>
+      <c r="B60" t="s">
+        <v>46</v>
+      </c>
+      <c r="C60">
+        <v>12</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>95</v>
+      </c>
+      <c r="F60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61">
+        <v>85</v>
+      </c>
+      <c r="B61" t="s">
+        <v>46</v>
+      </c>
+      <c r="C61">
+        <v>6</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>95</v>
+      </c>
+      <c r="F61" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62">
+        <v>86</v>
+      </c>
+      <c r="B62" t="s">
+        <v>48</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>95</v>
+      </c>
+      <c r="F62" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63">
+        <v>87</v>
+      </c>
+      <c r="B63" t="s">
+        <v>48</v>
+      </c>
+      <c r="C63">
+        <v>19</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>95</v>
+      </c>
+      <c r="F63" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64">
+        <v>88</v>
+      </c>
+      <c r="B64" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>95</v>
+      </c>
+      <c r="F64" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65">
+        <v>89</v>
+      </c>
+      <c r="B65" t="s">
+        <v>50</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>95</v>
+      </c>
+      <c r="F65" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66">
+        <v>90</v>
+      </c>
+      <c r="B66" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>95</v>
+      </c>
+      <c r="F66" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67">
+        <v>91</v>
+      </c>
+      <c r="B67" t="s">
+        <v>51</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>95</v>
+      </c>
+      <c r="F67" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68">
+        <v>93</v>
+      </c>
+      <c r="B68" t="s">
+        <v>52</v>
+      </c>
+      <c r="C68">
+        <v>14</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>95</v>
+      </c>
+      <c r="F68" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69">
+        <v>94</v>
+      </c>
+      <c r="B69" t="s">
+        <v>53</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>95</v>
+      </c>
+      <c r="F69" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70">
+        <v>95</v>
+      </c>
+      <c r="B70" t="s">
+        <v>53</v>
+      </c>
+      <c r="C70">
+        <v>10</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>95</v>
+      </c>
+      <c r="F70" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71">
+        <v>96</v>
+      </c>
+      <c r="B71" t="s">
+        <v>53</v>
+      </c>
+      <c r="C71">
+        <v>12</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>95</v>
+      </c>
+      <c r="F71" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72">
+        <v>97</v>
+      </c>
+      <c r="B72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C72">
+        <v>16</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>95</v>
+      </c>
+      <c r="F72" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73">
+        <v>99</v>
+      </c>
+      <c r="B73" t="s">
+        <v>56</v>
+      </c>
+      <c r="C73">
+        <v>18</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>95</v>
+      </c>
+      <c r="F73" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74">
+        <v>100</v>
+      </c>
+      <c r="B74" t="s">
+        <v>57</v>
+      </c>
+      <c r="C74">
+        <v>14</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>95</v>
+      </c>
+      <c r="F74" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75">
+        <v>101</v>
+      </c>
+      <c r="B75" t="s">
+        <v>58</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>95</v>
+      </c>
+      <c r="F75" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76">
+        <v>102</v>
+      </c>
+      <c r="B76" t="s">
+        <v>59</v>
+      </c>
+      <c r="C76">
+        <v>10</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>95</v>
+      </c>
+      <c r="F76" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77">
+        <v>103</v>
+      </c>
+      <c r="B77" t="s">
+        <v>60</v>
+      </c>
+      <c r="C77">
+        <v>10</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>95</v>
+      </c>
+      <c r="F77" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78">
+        <v>104</v>
+      </c>
+      <c r="B78" t="s">
+        <v>61</v>
+      </c>
+      <c r="C78">
+        <v>14</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>95</v>
+      </c>
+      <c r="F78" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79">
+        <v>105</v>
+      </c>
+      <c r="B79" t="s">
+        <v>62</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>95</v>
+      </c>
+      <c r="F79" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80">
+        <v>106</v>
+      </c>
+      <c r="B80" t="s">
+        <v>63</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>95</v>
+      </c>
+      <c r="F80" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81">
+        <v>107</v>
+      </c>
+      <c r="B81" t="s">
+        <v>64</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>95</v>
+      </c>
+      <c r="F81" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82">
+        <v>108</v>
+      </c>
+      <c r="B82" t="s">
+        <v>64</v>
+      </c>
+      <c r="C82">
+        <v>4</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>95</v>
+      </c>
+      <c r="F82" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83">
+        <v>109</v>
+      </c>
+      <c r="B83" t="s">
+        <v>66</v>
+      </c>
+      <c r="C83">
+        <v>5</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>95</v>
+      </c>
+      <c r="F83" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="A84">
+        <v>110</v>
+      </c>
+      <c r="B84" t="s">
+        <v>67</v>
+      </c>
+      <c r="C84">
+        <v>18</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>95</v>
+      </c>
+      <c r="F84" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="A85">
+        <v>111</v>
+      </c>
+      <c r="B85" t="s">
+        <v>68</v>
+      </c>
+      <c r="C85">
+        <v>14</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>95</v>
+      </c>
+      <c r="F85" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="A86">
+        <v>112</v>
+      </c>
+      <c r="B86" t="s">
+        <v>69</v>
+      </c>
+      <c r="C86">
+        <v>16</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <v>95</v>
+      </c>
+      <c r="F86" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="A87">
+        <v>113</v>
+      </c>
+      <c r="B87" t="s">
+        <v>69</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>95</v>
+      </c>
+      <c r="F87" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
+      <c r="A88">
+        <v>114</v>
+      </c>
+      <c r="B88" t="s">
+        <v>70</v>
+      </c>
+      <c r="C88">
+        <v>12</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>95</v>
+      </c>
+      <c r="F88" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
+      <c r="A89">
+        <v>115</v>
+      </c>
+      <c r="B89" t="s">
+        <v>71</v>
+      </c>
+      <c r="C89">
+        <v>9</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>95</v>
+      </c>
+      <c r="F89" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
+      <c r="A90">
+        <v>116</v>
+      </c>
+      <c r="B90" t="s">
+        <v>72</v>
+      </c>
+      <c r="C90">
+        <v>19</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>95</v>
+      </c>
+      <c r="F90" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
+      <c r="A91">
+        <v>118</v>
+      </c>
+      <c r="B91" t="s">
+        <v>73</v>
+      </c>
+      <c r="C91">
+        <v>16</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>95</v>
+      </c>
+      <c r="F91" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
+      <c r="A92">
+        <v>119</v>
+      </c>
+      <c r="B92" t="s">
+        <v>73</v>
+      </c>
+      <c r="C92">
+        <v>18</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <v>95</v>
+      </c>
+      <c r="F92" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="A93">
+        <v>120</v>
+      </c>
+      <c r="B93" t="s">
+        <v>73</v>
+      </c>
+      <c r="C93">
+        <v>14</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>95</v>
+      </c>
+      <c r="F93" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94">
+        <v>121</v>
+      </c>
+      <c r="B94" t="s">
+        <v>73</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94">
+        <v>95</v>
+      </c>
+      <c r="F94" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="A95">
+        <v>122</v>
+      </c>
+      <c r="B95" t="s">
+        <v>75</v>
+      </c>
+      <c r="C95">
+        <v>14</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95">
+        <v>95</v>
+      </c>
+      <c r="F95" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="A96">
+        <v>123</v>
+      </c>
+      <c r="B96" t="s">
+        <v>76</v>
+      </c>
+      <c r="C96">
+        <v>19</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>95</v>
+      </c>
+      <c r="F96" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
+      <c r="A97">
+        <v>124</v>
+      </c>
+      <c r="B97" t="s">
+        <v>77</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>95</v>
+      </c>
+      <c r="F97" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
+      <c r="A98">
+        <v>125</v>
+      </c>
+      <c r="B98" t="s">
+        <v>77</v>
+      </c>
+      <c r="C98">
+        <v>16</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>95</v>
+      </c>
+      <c r="F98" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
+      <c r="A99">
+        <v>126</v>
+      </c>
+      <c r="B99" t="s">
+        <v>78</v>
+      </c>
+      <c r="C99">
+        <v>3</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>95</v>
+      </c>
+      <c r="F99" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
+      <c r="A100">
+        <v>127</v>
+      </c>
+      <c r="B100" t="s">
+        <v>79</v>
+      </c>
+      <c r="C100">
+        <v>18</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="E100">
+        <v>95</v>
+      </c>
+      <c r="F100" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
+      <c r="A101">
+        <v>128</v>
+      </c>
+      <c r="B101" t="s">
+        <v>72</v>
+      </c>
+      <c r="C101">
+        <v>3</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>95</v>
+      </c>
+      <c r="F101" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
+      <c r="A102">
+        <v>129</v>
+      </c>
+      <c r="B102" t="s">
+        <v>81</v>
+      </c>
+      <c r="C102">
+        <v>16</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>95</v>
+      </c>
+      <c r="F102" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
+      <c r="A103">
+        <v>130</v>
+      </c>
+      <c r="B103" t="s">
+        <v>82</v>
+      </c>
+      <c r="C103">
+        <v>12</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103">
+        <v>95</v>
+      </c>
+      <c r="F103" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
+      <c r="A104">
+        <v>131</v>
+      </c>
+      <c r="B104" t="s">
+        <v>82</v>
+      </c>
+      <c r="C104">
+        <v>3</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104">
+        <v>95</v>
+      </c>
+      <c r="F104" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
+      <c r="A105">
+        <v>132</v>
+      </c>
+      <c r="B105" t="s">
+        <v>83</v>
+      </c>
+      <c r="C105">
+        <v>4</v>
+      </c>
+      <c r="D105">
+        <v>1</v>
+      </c>
+      <c r="E105">
+        <v>95</v>
+      </c>
+      <c r="F105" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
+      <c r="A106">
+        <v>133</v>
+      </c>
+      <c r="B106" t="s">
+        <v>83</v>
+      </c>
+      <c r="C106">
+        <v>18</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106">
+        <v>95</v>
+      </c>
+      <c r="F106" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
+      <c r="A107">
+        <v>134</v>
+      </c>
+      <c r="B107" t="s">
+        <v>84</v>
+      </c>
+      <c r="C107">
+        <v>5</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <v>95</v>
+      </c>
+      <c r="F107" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
+      <c r="A108">
+        <v>135</v>
+      </c>
+      <c r="B108" t="s">
+        <v>84</v>
+      </c>
+      <c r="C108">
+        <v>19</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108">
+        <v>95</v>
+      </c>
+      <c r="F108" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
+      <c r="A109">
+        <v>136</v>
+      </c>
+      <c r="B109" t="s">
+        <v>85</v>
+      </c>
+      <c r="C109">
+        <v>18</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109">
+        <v>95</v>
+      </c>
+      <c r="F109" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
+      <c r="A110">
+        <v>137</v>
+      </c>
+      <c r="B110" t="s">
+        <v>86</v>
+      </c>
+      <c r="C110">
+        <v>14</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110">
+        <v>95</v>
+      </c>
+      <c r="F110" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se esta haciendo el diseño
</commit_message>
<xml_diff>
--- a/excel/aceites.xlsx
+++ b/excel/aceites.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="104">
   <si>
     <t>ID</t>
   </si>
@@ -73,15 +73,18 @@
     <t>2025-01-21</t>
   </si>
   <si>
+    <t>oswi</t>
+  </si>
+  <si>
+    <t>planta</t>
+  </si>
+  <si>
     <t>2025-01-22</t>
   </si>
   <si>
     <t>2025-01-23</t>
   </si>
   <si>
-    <t>planta</t>
-  </si>
-  <si>
     <t>IWAED389881</t>
   </si>
   <si>
@@ -115,9 +118,6 @@
     <t>2025-02-05</t>
   </si>
   <si>
-    <t>oswi</t>
-  </si>
-  <si>
     <t>2025-02-06</t>
   </si>
   <si>
@@ -278,6 +278,57 @@
   </si>
   <si>
     <t>2025-05-12</t>
+  </si>
+  <si>
+    <t>2025-05-13</t>
+  </si>
+  <si>
+    <t>IWAED397702</t>
+  </si>
+  <si>
+    <t>2025-05-14</t>
+  </si>
+  <si>
+    <t>2025-05-15</t>
+  </si>
+  <si>
+    <t>2025-05-17</t>
+  </si>
+  <si>
+    <t>2025-05-25</t>
+  </si>
+  <si>
+    <t>2025-05-27</t>
+  </si>
+  <si>
+    <t>2025-05-30</t>
+  </si>
+  <si>
+    <t>2025-06-02</t>
+  </si>
+  <si>
+    <t>IWAED399333</t>
+  </si>
+  <si>
+    <t>2025-06-03</t>
+  </si>
+  <si>
+    <t>2025-06-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IWAED399333</t>
+  </si>
+  <si>
+    <t>2025-06-05</t>
+  </si>
+  <si>
+    <t>2025-06-06</t>
+  </si>
+  <si>
+    <t>2025-06-07</t>
+  </si>
+  <si>
+    <t>2025-06-09</t>
   </si>
 </sst>
 </file>
@@ -640,7 +691,7 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L110"/>
+  <dimension ref="A1:L136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="N8" sqref="N8"/>
@@ -1082,7 +1133,7 @@
         <v>16</v>
       </c>
       <c r="J15" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -1111,7 +1162,7 @@
         <v>16</v>
       </c>
       <c r="J16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -1125,7 +1176,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -1145,7 +1196,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>10</v>
@@ -1165,7 +1216,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>14</v>
@@ -1185,7 +1236,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1205,10 +1256,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
         <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1225,7 +1276,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>10</v>
@@ -1237,7 +1288,7 @@
         <v>93</v>
       </c>
       <c r="F22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1245,7 +1296,7 @@
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23">
         <v>6</v>
@@ -1257,7 +1308,7 @@
         <v>93</v>
       </c>
       <c r="F23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1265,7 +1316,7 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>10</v>
@@ -1277,7 +1328,7 @@
         <v>93</v>
       </c>
       <c r="F24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1285,7 +1336,7 @@
         <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -1297,7 +1348,7 @@
         <v>93</v>
       </c>
       <c r="F25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1305,7 +1356,7 @@
         <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C26">
         <v>6</v>
@@ -1317,7 +1368,7 @@
         <v>93</v>
       </c>
       <c r="F26" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1325,7 +1376,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1337,7 +1388,7 @@
         <v>93</v>
       </c>
       <c r="F27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1345,7 +1396,7 @@
         <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C28">
         <v>10</v>
@@ -1357,7 +1408,7 @@
         <v>93</v>
       </c>
       <c r="F28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1365,7 +1416,7 @@
         <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C29">
         <v>14</v>
@@ -1377,7 +1428,7 @@
         <v>93</v>
       </c>
       <c r="F29" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1385,7 +1436,7 @@
         <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1397,7 +1448,7 @@
         <v>93</v>
       </c>
       <c r="F30" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1405,7 +1456,7 @@
         <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C31">
         <v>10</v>
@@ -1417,7 +1468,7 @@
         <v>93</v>
       </c>
       <c r="F31" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1425,7 +1476,7 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C32">
         <v>10</v>
@@ -1437,7 +1488,7 @@
         <v>93</v>
       </c>
       <c r="F32" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1445,7 +1496,7 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C33">
         <v>10</v>
@@ -1457,7 +1508,7 @@
         <v>93</v>
       </c>
       <c r="F33" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1465,7 +1516,7 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C34">
         <v>12</v>
@@ -1477,7 +1528,7 @@
         <v>93</v>
       </c>
       <c r="F34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1485,7 +1536,7 @@
         <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -1497,7 +1548,7 @@
         <v>93</v>
       </c>
       <c r="F35" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1505,7 +1556,7 @@
         <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1517,7 +1568,7 @@
         <v>93</v>
       </c>
       <c r="F36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1525,7 +1576,7 @@
         <v>50</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1537,7 +1588,7 @@
         <v>93</v>
       </c>
       <c r="F37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1545,7 +1596,7 @@
         <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C38">
         <v>10</v>
@@ -1557,7 +1608,7 @@
         <v>93</v>
       </c>
       <c r="F38" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -1565,7 +1616,7 @@
         <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C39">
         <v>6</v>
@@ -1577,7 +1628,7 @@
         <v>93</v>
       </c>
       <c r="F39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -1585,7 +1636,7 @@
         <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1597,7 +1648,7 @@
         <v>93</v>
       </c>
       <c r="F40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -1605,10 +1656,10 @@
         <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -1617,7 +1668,7 @@
         <v>93</v>
       </c>
       <c r="F41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2998,6 +3049,526 @@
       </c>
       <c r="F110" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12">
+      <c r="A111">
+        <v>138</v>
+      </c>
+      <c r="B111" t="s">
+        <v>87</v>
+      </c>
+      <c r="C111">
+        <v>16</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111">
+        <v>95</v>
+      </c>
+      <c r="F111" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
+      <c r="A112">
+        <v>139</v>
+      </c>
+      <c r="B112" t="s">
+        <v>87</v>
+      </c>
+      <c r="C112">
+        <v>3</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112">
+        <v>95</v>
+      </c>
+      <c r="F112" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
+      <c r="A113">
+        <v>140</v>
+      </c>
+      <c r="B113" t="s">
+        <v>89</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113">
+        <v>95</v>
+      </c>
+      <c r="F113" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
+      <c r="A114">
+        <v>141</v>
+      </c>
+      <c r="B114" t="s">
+        <v>90</v>
+      </c>
+      <c r="C114">
+        <v>18</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114">
+        <v>95</v>
+      </c>
+      <c r="F114" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
+      <c r="A115">
+        <v>142</v>
+      </c>
+      <c r="B115" t="s">
+        <v>91</v>
+      </c>
+      <c r="C115">
+        <v>14</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+      <c r="E115">
+        <v>95</v>
+      </c>
+      <c r="F115" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
+      <c r="A116">
+        <v>143</v>
+      </c>
+      <c r="B116" t="s">
+        <v>92</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116">
+        <v>95</v>
+      </c>
+      <c r="F116" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
+      <c r="A117">
+        <v>145</v>
+      </c>
+      <c r="B117" t="s">
+        <v>91</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117">
+        <v>95</v>
+      </c>
+      <c r="F117" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
+      <c r="A118">
+        <v>146</v>
+      </c>
+      <c r="B118" t="s">
+        <v>93</v>
+      </c>
+      <c r="C118">
+        <v>3</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118">
+        <v>95</v>
+      </c>
+      <c r="F118" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
+      <c r="A119">
+        <v>147</v>
+      </c>
+      <c r="B119" t="s">
+        <v>93</v>
+      </c>
+      <c r="C119">
+        <v>4</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="E119">
+        <v>95</v>
+      </c>
+      <c r="F119" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="A120">
+        <v>148</v>
+      </c>
+      <c r="B120" t="s">
+        <v>94</v>
+      </c>
+      <c r="C120">
+        <v>16</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120">
+        <v>95</v>
+      </c>
+      <c r="F120" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
+      <c r="A121">
+        <v>149</v>
+      </c>
+      <c r="B121" t="s">
+        <v>95</v>
+      </c>
+      <c r="C121">
+        <v>18</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+      <c r="E121">
+        <v>95</v>
+      </c>
+      <c r="F121" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
+      <c r="A122">
+        <v>151</v>
+      </c>
+      <c r="B122" t="s">
+        <v>97</v>
+      </c>
+      <c r="C122">
+        <v>3</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122">
+        <v>95</v>
+      </c>
+      <c r="F122" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
+      <c r="A123">
+        <v>152</v>
+      </c>
+      <c r="B123" t="s">
+        <v>97</v>
+      </c>
+      <c r="C123">
+        <v>1</v>
+      </c>
+      <c r="D123">
+        <v>2</v>
+      </c>
+      <c r="E123">
+        <v>95</v>
+      </c>
+      <c r="F123" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
+      <c r="A124">
+        <v>153</v>
+      </c>
+      <c r="B124" t="s">
+        <v>98</v>
+      </c>
+      <c r="C124">
+        <v>6</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124">
+        <v>95</v>
+      </c>
+      <c r="F124" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12">
+      <c r="A125">
+        <v>154</v>
+      </c>
+      <c r="B125" t="s">
+        <v>98</v>
+      </c>
+      <c r="C125">
+        <v>3</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+      <c r="E125">
+        <v>95</v>
+      </c>
+      <c r="F125" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12">
+      <c r="A126">
+        <v>158</v>
+      </c>
+      <c r="B126" t="s">
+        <v>95</v>
+      </c>
+      <c r="C126">
+        <v>18</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+      <c r="E126">
+        <v>95</v>
+      </c>
+      <c r="F126" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12">
+      <c r="A127">
+        <v>159</v>
+      </c>
+      <c r="B127" t="s">
+        <v>97</v>
+      </c>
+      <c r="C127">
+        <v>3</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="E127">
+        <v>95</v>
+      </c>
+      <c r="F127" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12">
+      <c r="A128">
+        <v>161</v>
+      </c>
+      <c r="B128" t="s">
+        <v>95</v>
+      </c>
+      <c r="C128">
+        <v>18</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+      <c r="E128">
+        <v>95</v>
+      </c>
+      <c r="F128" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
+      <c r="A129">
+        <v>162</v>
+      </c>
+      <c r="B129" t="s">
+        <v>97</v>
+      </c>
+      <c r="C129">
+        <v>3</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+      <c r="E129">
+        <v>95</v>
+      </c>
+      <c r="F129" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
+      <c r="A130">
+        <v>163</v>
+      </c>
+      <c r="B130" t="s">
+        <v>97</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
+      </c>
+      <c r="E130">
+        <v>95</v>
+      </c>
+      <c r="F130" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
+      <c r="A131">
+        <v>165</v>
+      </c>
+      <c r="B131" t="s">
+        <v>98</v>
+      </c>
+      <c r="C131">
+        <v>6</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+      <c r="E131">
+        <v>95</v>
+      </c>
+      <c r="F131" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
+      <c r="A132">
+        <v>166</v>
+      </c>
+      <c r="B132" t="s">
+        <v>100</v>
+      </c>
+      <c r="C132">
+        <v>3</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+      <c r="E132">
+        <v>95</v>
+      </c>
+      <c r="F132" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
+      <c r="A133">
+        <v>167</v>
+      </c>
+      <c r="B133" t="s">
+        <v>101</v>
+      </c>
+      <c r="C133">
+        <v>10</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+      <c r="E133">
+        <v>95</v>
+      </c>
+      <c r="F133" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
+      <c r="A134">
+        <v>168</v>
+      </c>
+      <c r="B134" t="s">
+        <v>102</v>
+      </c>
+      <c r="C134">
+        <v>12</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+      <c r="E134">
+        <v>95</v>
+      </c>
+      <c r="F134" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
+      <c r="A135">
+        <v>169</v>
+      </c>
+      <c r="B135" t="s">
+        <v>102</v>
+      </c>
+      <c r="C135">
+        <v>14</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+      <c r="E135">
+        <v>95</v>
+      </c>
+      <c r="F135" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
+      <c r="A136">
+        <v>170</v>
+      </c>
+      <c r="B136" t="s">
+        <v>103</v>
+      </c>
+      <c r="C136">
+        <v>18</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="E136">
+        <v>95</v>
+      </c>
+      <c r="F136" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agrego el download_informe y se cambiaron los nombres de los archivos y se termino el archivo de buscar
</commit_message>
<xml_diff>
--- a/excel/aceites.xlsx
+++ b/excel/aceites.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\AceitesSufa\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CAFE9D-F69D-4750-A55A-CFD7400EABA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja1'!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$L$1</definedName>
   </definedNames>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="999999"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="104">
   <si>
     <t>ID</t>
   </si>
@@ -334,24 +340,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -385,19 +382,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -687,24 +692,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="J138" sqref="J138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="9.140625" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" customWidth="true" style="0"/>
-    <col min="6" max="6" width="18" customWidth="true" style="0"/>
-    <col min="9" max="9" width="11.85546875" customWidth="true" style="0"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -736,7 +738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -765,7 +767,7 @@
         <v>2169</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -794,7 +796,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -823,7 +825,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -852,7 +854,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -881,7 +883,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -910,7 +912,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -939,7 +941,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -968,7 +970,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -997,7 +999,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1026,7 +1028,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1055,7 +1057,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1084,7 +1086,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1113,7 +1115,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1142,7 +1144,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1171,7 +1173,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1191,7 +1193,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1211,7 +1213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1231,7 +1233,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1251,7 +1253,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1271,7 +1273,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>30</v>
       </c>
@@ -1291,7 +1293,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>31</v>
       </c>
@@ -1311,7 +1313,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>32</v>
       </c>
@@ -1331,7 +1333,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>33</v>
       </c>
@@ -1351,7 +1353,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>34</v>
       </c>
@@ -1371,7 +1373,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>35</v>
       </c>
@@ -1391,7 +1393,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>36</v>
       </c>
@@ -1411,7 +1413,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>37</v>
       </c>
@@ -1431,7 +1433,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>38</v>
       </c>
@@ -1451,7 +1453,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>39</v>
       </c>
@@ -1471,7 +1473,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>44</v>
       </c>
@@ -1491,7 +1493,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>45</v>
       </c>
@@ -1511,7 +1513,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>46</v>
       </c>
@@ -1531,7 +1533,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>47</v>
       </c>
@@ -1551,7 +1553,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>48</v>
       </c>
@@ -1571,7 +1573,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>50</v>
       </c>
@@ -1591,7 +1593,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>51</v>
       </c>
@@ -1611,7 +1613,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>52</v>
       </c>
@@ -1631,7 +1633,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>53</v>
       </c>
@@ -1651,7 +1653,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>54</v>
       </c>
@@ -1671,7 +1673,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>65</v>
       </c>
@@ -1691,7 +1693,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>66</v>
       </c>
@@ -1711,7 +1713,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>67</v>
       </c>
@@ -1731,7 +1733,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>68</v>
       </c>
@@ -1751,7 +1753,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>69</v>
       </c>
@@ -1771,7 +1773,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>70</v>
       </c>
@@ -1791,7 +1793,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>71</v>
       </c>
@@ -1811,7 +1813,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>72</v>
       </c>
@@ -1831,7 +1833,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>73</v>
       </c>
@@ -1851,7 +1853,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>74</v>
       </c>
@@ -1871,7 +1873,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>75</v>
       </c>
@@ -1891,7 +1893,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>77</v>
       </c>
@@ -1911,7 +1913,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>78</v>
       </c>
@@ -1931,7 +1933,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>79</v>
       </c>
@@ -1951,7 +1953,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>80</v>
       </c>
@@ -1971,7 +1973,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>81</v>
       </c>
@@ -1991,7 +1993,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>82</v>
       </c>
@@ -2011,7 +2013,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>83</v>
       </c>
@@ -2031,7 +2033,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>84</v>
       </c>
@@ -2051,7 +2053,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>85</v>
       </c>
@@ -2071,7 +2073,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>86</v>
       </c>
@@ -2091,7 +2093,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>87</v>
       </c>
@@ -2111,7 +2113,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>88</v>
       </c>
@@ -2131,7 +2133,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>89</v>
       </c>
@@ -2151,7 +2153,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>90</v>
       </c>
@@ -2171,7 +2173,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>91</v>
       </c>
@@ -2191,7 +2193,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>93</v>
       </c>
@@ -2211,7 +2213,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>94</v>
       </c>
@@ -2231,7 +2233,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>95</v>
       </c>
@@ -2251,7 +2253,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>96</v>
       </c>
@@ -2271,7 +2273,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>97</v>
       </c>
@@ -2291,7 +2293,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>99</v>
       </c>
@@ -2311,7 +2313,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>100</v>
       </c>
@@ -2331,7 +2333,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>101</v>
       </c>
@@ -2351,7 +2353,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>102</v>
       </c>
@@ -2371,7 +2373,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>103</v>
       </c>
@@ -2391,7 +2393,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>104</v>
       </c>
@@ -2411,7 +2413,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>105</v>
       </c>
@@ -2431,7 +2433,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>106</v>
       </c>
@@ -2451,7 +2453,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>107</v>
       </c>
@@ -2471,7 +2473,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>108</v>
       </c>
@@ -2491,7 +2493,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>109</v>
       </c>
@@ -2511,7 +2513,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="84" spans="1:12">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>110</v>
       </c>
@@ -2531,7 +2533,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:12">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>111</v>
       </c>
@@ -2551,7 +2553,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="86" spans="1:12">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>112</v>
       </c>
@@ -2571,7 +2573,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:12">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>113</v>
       </c>
@@ -2591,7 +2593,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>114</v>
       </c>
@@ -2611,7 +2613,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>115</v>
       </c>
@@ -2631,7 +2633,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>116</v>
       </c>
@@ -2651,7 +2653,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="91" spans="1:12">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>118</v>
       </c>
@@ -2671,7 +2673,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>119</v>
       </c>
@@ -2691,7 +2693,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="93" spans="1:12">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>120</v>
       </c>
@@ -2711,7 +2713,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>121</v>
       </c>
@@ -2731,7 +2733,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:12">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>122</v>
       </c>
@@ -2751,7 +2753,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="96" spans="1:12">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>123</v>
       </c>
@@ -2771,7 +2773,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>124</v>
       </c>
@@ -2791,7 +2793,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="98" spans="1:12">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>125</v>
       </c>
@@ -2811,7 +2813,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="99" spans="1:12">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>126</v>
       </c>
@@ -2831,7 +2833,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:12">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>127</v>
       </c>
@@ -2851,7 +2853,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="101" spans="1:12">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>128</v>
       </c>
@@ -2871,7 +2873,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:12">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>129</v>
       </c>
@@ -2891,7 +2893,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:12">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>130</v>
       </c>
@@ -2911,7 +2913,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:12">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>131</v>
       </c>
@@ -2931,7 +2933,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="105" spans="1:12">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>132</v>
       </c>
@@ -2951,7 +2953,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="106" spans="1:12">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>133</v>
       </c>
@@ -2971,7 +2973,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="107" spans="1:12">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>134</v>
       </c>
@@ -2991,7 +2993,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="108" spans="1:12">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>135</v>
       </c>
@@ -3011,7 +3013,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="109" spans="1:12">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>136</v>
       </c>
@@ -3031,7 +3033,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="110" spans="1:12">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>137</v>
       </c>
@@ -3051,7 +3053,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="111" spans="1:12">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>138</v>
       </c>
@@ -3071,7 +3073,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="112" spans="1:12">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>139</v>
       </c>
@@ -3091,7 +3093,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="113" spans="1:12">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>140</v>
       </c>
@@ -3111,7 +3113,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="114" spans="1:12">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>141</v>
       </c>
@@ -3131,7 +3133,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="115" spans="1:12">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>142</v>
       </c>
@@ -3151,7 +3153,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="116" spans="1:12">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>143</v>
       </c>
@@ -3171,7 +3173,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>145</v>
       </c>
@@ -3191,7 +3193,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="118" spans="1:12">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>146</v>
       </c>
@@ -3211,7 +3213,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>147</v>
       </c>
@@ -3231,7 +3233,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>148</v>
       </c>
@@ -3251,7 +3253,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="121" spans="1:12">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>149</v>
       </c>
@@ -3271,7 +3273,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="122" spans="1:12">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>151</v>
       </c>
@@ -3291,7 +3293,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="123" spans="1:12">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>152</v>
       </c>
@@ -3311,7 +3313,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>153</v>
       </c>
@@ -3331,7 +3333,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="125" spans="1:12">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>154</v>
       </c>
@@ -3351,7 +3353,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="126" spans="1:12">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>158</v>
       </c>
@@ -3371,7 +3373,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="127" spans="1:12">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>159</v>
       </c>
@@ -3391,7 +3393,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="128" spans="1:12">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>161</v>
       </c>
@@ -3411,7 +3413,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="129" spans="1:12">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>162</v>
       </c>
@@ -3431,7 +3433,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="130" spans="1:12">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>163</v>
       </c>
@@ -3451,7 +3453,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="131" spans="1:12">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>165</v>
       </c>
@@ -3471,7 +3473,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="132" spans="1:12">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>166</v>
       </c>
@@ -3491,7 +3493,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="133" spans="1:12">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>167</v>
       </c>
@@ -3511,7 +3513,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="134" spans="1:12">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>168</v>
       </c>
@@ -3531,7 +3533,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="135" spans="1:12">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>169</v>
       </c>
@@ -3551,7 +3553,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="136" spans="1:12">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>170</v>
       </c>
@@ -3572,9 +3574,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <autoFilter ref="A1:L1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="187" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId1ps"/>
+  <pageSetup paperSize="187" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>